<commit_message>
Re-did 1NF, fixed a few issues with 2NF/3NF
</commit_message>
<xml_diff>
--- a/normalization_spreadsheet.xlsx
+++ b/normalization_spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebull_000\Dropbox\School\database_systems\Final Project\normalization_rough_drafts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebull_000\Dropbox\School\database_systems\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="53">
   <si>
     <t>date_created</t>
   </si>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>os.max_affected_version</t>
+  </si>
+  <si>
+    <t>min_affected_version</t>
+  </si>
+  <si>
+    <t>max_affected_version</t>
+  </si>
+  <si>
+    <t>application.min_affected_version</t>
+  </si>
+  <si>
+    <t>application.max_affected_version</t>
   </si>
 </sst>
 </file>
@@ -415,7 +427,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -435,6 +446,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22" customBuiltin="1"/>
@@ -751,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J124"/>
+  <dimension ref="A2:J145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124:B124"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136:C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,6 +1010,10 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1008,9 +1024,7 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
+      <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1022,9 +1036,12 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>12</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1034,15 +1051,6 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1056,10 +1064,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1070,14 +1078,14 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>27</v>
+      <c r="A22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1088,14 +1096,14 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>41</v>
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1106,15 +1114,6 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1124,14 +1123,14 @@
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>43</v>
+      <c r="A25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1142,14 +1141,8 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>36</v>
+      <c r="A26" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1160,15 +1153,6 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1178,14 +1162,14 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>19</v>
+      <c r="A28" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1196,15 +1180,17 @@
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A29" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1213,556 +1199,725 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="8" t="s">
+      <c r="C43" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>9</v>
+      <c r="C45" s="20" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="16" t="s">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C65" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B66" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C66" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B69" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C69" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B72" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C72" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C64" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>44</v>
+      <c r="A73" s="17" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B75" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>45</v>
+      <c r="B75" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>6</v>
+      <c r="C88" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>8</v>
+      <c r="A89" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B91" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
+      <c r="B95" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B94" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>26</v>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>11</v>
+      <c r="A99" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>35</v>
+      <c r="A105" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>40</v>
+      <c r="A108" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B112" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>11</v>
+      <c r="A112" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>45</v>
+      <c r="A115" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
-        <v>1</v>
+      <c r="A116" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B118" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>43</v>
+      <c r="B118" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
-        <v>44</v>
+      <c r="A119" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B121" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="B121" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C121" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B133" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="C133" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>